<commit_message>
Almost Finished Step 6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojns\Documents\DA8\Projects\budget_lookups-Jerspen175\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9B9D68-52E8-44F9-96D8-3AAD897D5C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969EB6FE-B856-484A-A977-D4EA3BF61D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10890" yWindow="135" windowWidth="19020" windowHeight="20730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4662,22 +4662,45 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="6">
+        <f>INDEX($A$2:$F$52, MATCH($B$87, $A$2:$A$52,0), 2)</f>
+        <v>7670700</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX($A$2:$F$52, MATCH($B$87, $A$2:$A$52,0), 3)</f>
+        <v>6947552.6699999999</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX($A$2:$K$52, MATCH($B$87, $A$2:$A$52,0), 2)</f>
+        <v>7670700</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" ref="C85:C86" si="15">INDEX($A$2:$F$52, MATCH($B$87, $A$2:$A$52,0), 3)</f>
+        <v>6947552.6699999999</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f t="shared" ref="B85:B86" si="16">INDEX($A$2:$P$52, MATCH($B$87, $A$2:$A$52,0), 2)</f>
+        <v>7670700</v>
+      </c>
+      <c r="C86" s="6">
+        <f t="shared" si="15"/>
+        <v>6947552.6699999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -4814,7 +4837,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>

</xml_diff>

<commit_message>
Fixed positivew values to negative
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojns\Documents\DA8\Projects\budget_lookups-Jerspen175\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC909018-70FC-42F4-9E04-DFC324DB930D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761D6E15-DA13-4B09-BC84-1C64E8AE4453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="270" windowWidth="19020" windowHeight="20730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="11955" windowHeight="20730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -2111,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,16 +2190,16 @@
         <v>341243679.13</v>
       </c>
       <c r="D2">
-        <f>IFERROR(B2-C2, 0)</f>
-        <v>15396420.870000005</v>
+        <f>IFERROR(C2-B2, 0)</f>
+        <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
         <f>IFERROR(D2/B2, 0)</f>
-        <v>4.3170750765267295E-2</v>
+        <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
         <f>_xlfn.RANK.EQ(E2, $E$2:$E$52, 0)</f>
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -2208,16 +2208,16 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f>IFERROR(G2-H2, 0)</f>
-        <v>36344389.180000007</v>
+        <f>IFERROR(H2-G2, 0)</f>
+        <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
         <f>IFERROR(I2/G2, 0)</f>
-        <v>9.4972027086493035E-2</v>
+        <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
         <f>_xlfn.RANK.EQ(J2, $J$2:$J$52, 0)</f>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -2226,16 +2226,16 @@
         <v>355279492.22999901</v>
       </c>
       <c r="N2">
-        <f>IFERROR(L2-M2, 0)</f>
-        <v>21269107.770000994</v>
+        <f>IFERROR(M2-L2, 0)</f>
+        <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
         <f>IFERROR(N2/L2, 0)</f>
-        <v>5.6484362894991494E-2</v>
+        <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
         <f>_xlfn.RANK.EQ(O2, $O$2:$O$52, 0)</f>
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2249,16 +2249,16 @@
         <v>321214.59000000003</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D52" si="0">IFERROR(B3-C3, 0)</f>
-        <v>7585.4099999999744</v>
+        <f t="shared" ref="D3:D52" si="0">IFERROR(C3-B3, 0)</f>
+        <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3, 0)</f>
-        <v>2.3069981751824741E-2</v>
+        <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3, $E$2:$E$52, 0)</f>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -2267,16 +2267,16 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I52" si="3">IFERROR(G3-H3, 0)</f>
-        <v>22366.290000001027</v>
+        <f t="shared" ref="I3:I52" si="3">IFERROR(H3-G3, 0)</f>
+        <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/G3, 0)</f>
-        <v>6.6804928315415249E-2</v>
+        <f>IFERROR(I3/G3, 0)</f>
+        <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3, $J$2:$J$52, 0)</f>
-        <v>14</v>
+        <f t="shared" ref="K3:K52" si="4">_xlfn.RANK.EQ(J3, $J$2:$J$52, 0)</f>
+        <v>38</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -2285,16 +2285,16 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="6">IFERROR(L3-M3, 0)</f>
-        <v>436.96000000002095</v>
+        <f t="shared" ref="N3:N52" si="5">IFERROR(M3-L3, 0)</f>
+        <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3, 0)</f>
-        <v>1.3540749922529313E-3</v>
+        <f t="shared" ref="O3:O52" si="6">IFERROR(N3/L3, 0)</f>
+        <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3, $O$2:$O$52, 0)</f>
-        <v>37</v>
+        <f t="shared" ref="P3:P52" si="7">_xlfn.RANK.EQ(O3, $O$2:$O$52, 0)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2309,15 +2309,15 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>15442.440000010189</v>
+        <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>4.9327413275443007E-3</v>
+        <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -2327,15 +2327,15 @@
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
-        <v>62606.790000009816</v>
+        <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" ref="J4:J52" si="8">IFERROR(I4/G4, 0)</f>
+        <v>-1.7141743558856015E-2</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="4"/>
-        <v>1.7141743558856015E-2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="5"/>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -2344,16 +2344,16 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
+        <f t="shared" si="5"/>
+        <v>-97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
         <f t="shared" si="6"/>
-        <v>97416.950000009965</v>
-      </c>
-      <c r="O4" s="5">
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="7"/>
-        <v>2.6599210899959033E-2</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="8"/>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2368,15 +2368,15 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>723147.33000000007</v>
+        <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>9.4273968477453174E-2</v>
+        <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -2386,15 +2386,15 @@
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>947690.6799999997</v>
+        <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.118932605449092</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="4"/>
-        <v>0.118932605449092</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -2403,16 +2403,16 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
+        <f t="shared" si="5"/>
+        <v>-262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
         <f t="shared" si="6"/>
-        <v>262277.08999999985</v>
-      </c>
-      <c r="O5" s="5">
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="7"/>
-        <v>3.3800336357544182E-2</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="8"/>
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2427,15 +2427,15 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>23391.479999999981</v>
+        <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>5.7149963352064452E-2</v>
+        <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -2445,15 +2445,15 @@
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>741.35999999998603</v>
+        <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.7301283547257551E-3</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="4"/>
-        <v>1.7301283547257551E-3</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="5"/>
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -2462,16 +2462,16 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
+        <f t="shared" si="5"/>
+        <v>-85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
         <f t="shared" si="6"/>
-        <v>85.710000001010485</v>
-      </c>
-      <c r="O6" s="5">
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="7"/>
-        <v>1.925202156356929E-4</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="8"/>
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2486,15 +2486,15 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>382928.79000000004</v>
+        <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>0.11502817362571344</v>
+        <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -2504,15 +2504,15 @@
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>339416.58999999985</v>
+        <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="4"/>
-        <v>0.10009631366303927</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -2521,16 +2521,16 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
+        <f t="shared" si="5"/>
+        <v>-398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
         <f t="shared" si="6"/>
-        <v>398759.91999999993</v>
-      </c>
-      <c r="O7" s="5">
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="7"/>
-        <v>0.11920361114432618</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2545,15 +2545,15 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>236476.69000000996</v>
+        <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="1"/>
-        <v>0.15235918433091292</v>
+        <v>-0.15235918433091292</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -2563,15 +2563,15 @@
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>206794.01000001002</v>
+        <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="4"/>
-        <v>0.13000189224870184</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -2580,16 +2580,16 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
+        <f t="shared" si="5"/>
+        <v>-241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
         <f t="shared" si="6"/>
-        <v>241564.68000000995</v>
-      </c>
-      <c r="O8" s="5">
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="7"/>
-        <v>0.15295680364719175</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2604,15 +2604,15 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>396574.72000000067</v>
+        <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>4.2417130511048909E-2</v>
+        <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -2622,15 +2622,15 @@
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>1144640.4800000004</v>
+        <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.10336567542917005</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="4"/>
-        <v>0.10336567542917005</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -2639,16 +2639,16 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
+        <f t="shared" si="5"/>
+        <v>-796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
         <f t="shared" si="6"/>
-        <v>796900.47000000998</v>
-      </c>
-      <c r="O9" s="5">
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="7"/>
-        <v>7.3852043000788653E-2</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2663,15 +2663,15 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>36209.630000000005</v>
+        <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>8.1681998646514792E-2</v>
+        <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -2681,15 +2681,15 @@
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>27292.159999999974</v>
+        <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="8"/>
+        <v>-5.5113408723747932E-2</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="4"/>
-        <v>5.5113408723747932E-2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -2698,16 +2698,16 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
+        <f t="shared" si="5"/>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
         <f t="shared" si="6"/>
-        <v>9181.0800000000163</v>
-      </c>
-      <c r="O10" s="5">
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="7"/>
-        <v>1.883298461538465E-2</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="8"/>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2743,12 +2743,12 @@
         <v>0</v>
       </c>
       <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="5"/>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -2757,16 +2757,16 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
+        <f t="shared" si="5"/>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="O11" s="5">
         <f t="shared" si="6"/>
-        <v>311228.08999999997</v>
-      </c>
-      <c r="O11" s="5">
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="7"/>
-        <v>0.82994157333333329</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2781,15 +2781,15 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>214304.66999999993</v>
+        <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>5.0060657805601608E-2</v>
+        <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -2799,15 +2799,15 @@
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>494844.40000000037</v>
+        <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.10527708280146378</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="4"/>
-        <v>0.10527708280146378</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -2816,16 +2816,16 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
         <f t="shared" si="6"/>
-        <v>306086.86000000034</v>
-      </c>
-      <c r="O12" s="5">
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="7"/>
-        <v>6.5433934755654441E-2</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2840,15 +2840,15 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>75511.669999999925</v>
+        <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="1"/>
-        <v>1.2912833886247806E-2</v>
+        <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -2858,15 +2858,15 @@
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>314622.06000000983</v>
+        <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>-5.0552253482656594E-2</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="4"/>
-        <v>5.0552253482656594E-2</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -2875,16 +2875,16 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
         <f t="shared" si="6"/>
-        <v>150323.33000000007</v>
-      </c>
-      <c r="O13" s="5">
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="7"/>
-        <v>2.4217184605222895E-2</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="8"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2899,15 +2899,15 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>6982.6300000000047</v>
+        <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="1"/>
-        <v>1.3637949218750009E-2</v>
+        <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2917,15 +2917,15 @@
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>6097.0200000000186</v>
+        <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.1492968897266765E-2</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="4"/>
-        <v>1.1492968897266765E-2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2934,16 +2934,16 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
+        <f t="shared" si="5"/>
+        <v>-21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
         <f t="shared" si="6"/>
-        <v>21210.119999999995</v>
-      </c>
-      <c r="O14" s="5">
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="7"/>
-        <v>4.0308095781071827E-2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2958,15 +2958,15 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>-496819.90000000596</v>
+        <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="1"/>
-        <v>-3.1837408866824991E-3</v>
+        <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2976,15 +2976,15 @@
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>8201410.7500010133</v>
+        <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.4532273014072019E-2</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="4"/>
-        <v>4.4532273014072019E-2</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2993,16 +2993,16 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
+        <f t="shared" si="5"/>
+        <v>-4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
         <f t="shared" si="6"/>
-        <v>4502589.1500009894</v>
-      </c>
-      <c r="O15" s="5">
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="7"/>
-        <v>2.3829085727446114E-2</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="8"/>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -3017,15 +3017,15 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>78219.540000010282</v>
+        <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="1"/>
-        <v>1.1850188616360429E-2</v>
+        <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -3035,15 +3035,15 @@
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>2035.9199999999255</v>
+        <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>-2.769017341040361E-4</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="4"/>
-        <v>2.769017341040361E-4</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -3052,16 +3052,16 @@
         <v>7397093</v>
       </c>
       <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-107</v>
+      </c>
+      <c r="O16" s="5">
         <f t="shared" si="6"/>
-        <v>107</v>
-      </c>
-      <c r="O16" s="5">
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="7"/>
-        <v>1.4464932677229222E-5</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="8"/>
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3076,15 +3076,15 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>421319.94999999925</v>
+        <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="1"/>
-        <v>2.8351094826658003E-2</v>
+        <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -3094,15 +3094,15 @@
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>664466.49000000022</v>
+        <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.3401666263871937E-2</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="4"/>
-        <v>4.3401666263871937E-2</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="5"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -3111,16 +3111,16 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
+        <f t="shared" si="5"/>
+        <v>-965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
         <f t="shared" si="6"/>
-        <v>965742.96000000089</v>
-      </c>
-      <c r="O17" s="5">
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="7"/>
-        <v>6.3071811282801551E-2</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="8"/>
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3135,15 +3135,15 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>149396.10000000987</v>
+        <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="1"/>
-        <v>5.4037002206391245E-2</v>
+        <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -3153,15 +3153,15 @@
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>189254.06000000006</v>
+        <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
+        <f t="shared" si="8"/>
+        <v>-6.6149619014330668E-2</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="4"/>
-        <v>6.6149619014330668E-2</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -3170,16 +3170,16 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
+        <f t="shared" si="5"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
         <f t="shared" si="6"/>
-        <v>374962.91000000015</v>
-      </c>
-      <c r="O18" s="5">
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="7"/>
-        <v>0.12882667147667154</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3194,15 +3194,15 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>376336.80000001006</v>
+        <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="1"/>
-        <v>4.258504294298146E-2</v>
+        <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -3212,15 +3212,15 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>721592.76000000909</v>
+        <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
+        <f t="shared" si="8"/>
+        <v>-7.4289145810384635E-2</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="4"/>
-        <v>7.4289145810384635E-2</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -3229,16 +3229,16 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
         <f t="shared" si="6"/>
-        <v>576344.08999999985</v>
-      </c>
-      <c r="O19" s="5">
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="7"/>
-        <v>6.1687262121374278E-2</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="8"/>
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3253,15 +3253,15 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1539.8400010019541</v>
+        <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="1"/>
-        <v>1.2379538203300809E-5</v>
+        <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -3271,15 +3271,15 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>9775.6299999952316</v>
+        <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
+        <f t="shared" si="8"/>
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="4"/>
-        <v>7.4142392760188761E-5</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="5"/>
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -3288,16 +3288,16 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
         <f t="shared" si="6"/>
-        <v>116.46000100672245</v>
-      </c>
-      <c r="O20" s="5">
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="7"/>
-        <v>8.9158438821450736E-7</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="8"/>
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3312,15 +3312,15 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>1923512.4500000998</v>
+        <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="1"/>
-        <v>7.9052463618023094E-2</v>
+        <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -3330,15 +3330,15 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>1841406.370000001</v>
+        <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
+        <f t="shared" si="8"/>
+        <v>-7.5167420624229556E-2</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="4"/>
-        <v>7.5167420624229556E-2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -3347,16 +3347,16 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
         <f t="shared" si="6"/>
-        <v>888926.91000010073</v>
-      </c>
-      <c r="O21" s="5">
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="7"/>
-        <v>3.6546762734864152E-2</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="8"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3371,15 +3371,15 @@
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>153660.12000009976</v>
+        <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="1"/>
-        <v>1.3285502334437123E-2</v>
+        <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -3389,15 +3389,15 @@
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>188722.03000009991</v>
+        <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.5752170574348738E-2</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="4"/>
-        <v>1.5752170574348738E-2</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -3406,16 +3406,16 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
+        <f t="shared" si="5"/>
+        <v>-745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
         <f t="shared" si="6"/>
-        <v>745.23000000044703</v>
-      </c>
-      <c r="O22" s="5">
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="7"/>
-        <v>6.2439674240938325E-5</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="8"/>
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3430,15 +3430,15 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>825956.59000010043</v>
+        <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>3.9590110100806722E-2</v>
+        <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -3448,14 +3448,14 @@
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>961673.78000010177</v>
+        <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.2394738976719144E-2</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="4"/>
-        <v>4.2394738976719144E-2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="L23">
@@ -3465,15 +3465,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
+        <f t="shared" si="5"/>
+        <v>-601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>601242.55999999866</v>
-      </c>
-      <c r="O23" s="5">
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="7"/>
-        <v>2.5892971236375011E-2</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="8"/>
         <v>26</v>
       </c>
     </row>
@@ -3489,15 +3489,15 @@
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>12230.810000000056</v>
+        <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="1"/>
-        <v>1.3334943305713101E-2</v>
+        <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -3507,15 +3507,15 @@
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>45485.580000000075</v>
+        <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.087856565111897E-2</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="4"/>
-        <v>4.087856565111897E-2</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -3524,16 +3524,16 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
+        <f t="shared" si="5"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
         <f t="shared" si="6"/>
-        <v>72.879999999888241</v>
-      </c>
-      <c r="O24" s="5">
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="7"/>
-        <v>6.5504224339284781E-5</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="8"/>
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3548,15 +3548,15 @@
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>4950.4699999999721</v>
+        <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="1"/>
-        <v>1.0226130964676661E-2</v>
+        <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -3566,15 +3566,15 @@
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>8005.7900000010268</v>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.5846773555029746E-2</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="4"/>
-        <v>1.5846773555029746E-2</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="5"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -3583,16 +3583,16 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
+        <f t="shared" si="5"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
         <f t="shared" si="6"/>
-        <v>1724.9000000000233</v>
-      </c>
-      <c r="O25" s="5">
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="7"/>
-        <v>3.4741188318228064E-3</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="8"/>
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3607,15 +3607,15 @@
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>447839.91999999993</v>
+        <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
         <f t="shared" si="1"/>
-        <v>8.5306091660634673E-2</v>
+        <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -3625,15 +3625,15 @@
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>319870.97000000998</v>
+        <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
+        <f t="shared" si="8"/>
+        <v>-5.8776040939327839E-2</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="4"/>
-        <v>5.8776040939327839E-2</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -3642,16 +3642,16 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
         <f t="shared" si="6"/>
-        <v>313464.79000000004</v>
-      </c>
-      <c r="O26" s="5">
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="7"/>
-        <v>5.7720881286022069E-2</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="8"/>
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -3687,30 +3687,30 @@
         <v>0</v>
       </c>
       <c r="J27" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5">
+      <c r="P27">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="8"/>
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3725,15 +3725,15 @@
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>132457.97999999998</v>
+        <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" si="1"/>
-        <v>9.5782760864849215E-2</v>
+        <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -3743,15 +3743,15 @@
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>264364.77</v>
+        <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="4"/>
-        <v>0.17103239309050916</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -3760,16 +3760,16 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
+        <f t="shared" si="5"/>
+        <v>-132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
         <f t="shared" si="6"/>
-        <v>132614.93999999994</v>
-      </c>
-      <c r="O28" s="5">
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="7"/>
-        <v>8.6909325643882263E-2</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3784,15 +3784,15 @@
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>37915.290000000037</v>
+        <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="1"/>
-        <v>1.4800253727847622E-2</v>
+        <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -3802,15 +3802,15 @@
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>114235.56000000983</v>
+        <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.1099320021590155E-2</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="4"/>
-        <v>4.1099320021590155E-2</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="5"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -3819,16 +3819,16 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
+        <f t="shared" si="5"/>
+        <v>-35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
         <f t="shared" si="6"/>
-        <v>35.330000000074506</v>
-      </c>
-      <c r="O29" s="5">
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="7"/>
-        <v>1.2225336516860273E-5</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="8"/>
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3843,15 +3843,15 @@
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>101705.90000000037</v>
+        <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
         <f t="shared" si="1"/>
-        <v>8.3831374359143746E-3</v>
+        <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -3861,15 +3861,15 @@
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>50385.720000099391</v>
+        <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.9561962641116366E-3</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="4"/>
-        <v>3.9561962641116366E-3</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="5"/>
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -3878,16 +3878,16 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
+        <f t="shared" si="5"/>
+        <v>-35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
         <f t="shared" si="6"/>
-        <v>35290.390000000596</v>
-      </c>
-      <c r="O30" s="5">
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="7"/>
-        <v>2.7439209100169185E-3</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="8"/>
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3902,15 +3902,15 @@
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>24772.310000000056</v>
+        <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
         <f t="shared" si="1"/>
-        <v>1.4030533529678329E-2</v>
+        <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3920,15 +3920,15 @@
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
-        <v>60623.149999999907</v>
+        <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.3249136181648611E-2</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="4"/>
-        <v>3.3249136181648611E-2</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="5"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3937,16 +3937,16 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
+        <f t="shared" si="5"/>
+        <v>-69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
         <f t="shared" si="6"/>
-        <v>69308.659999999916</v>
-      </c>
-      <c r="O31" s="5">
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="7"/>
-        <v>3.7049585716576634E-2</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3961,15 +3961,15 @@
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>73762.280000009574</v>
+        <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="1"/>
-        <v>1.2294942827617691E-2</v>
+        <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3979,15 +3979,15 @@
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>110514.53000000026</v>
+        <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.7837871035428981E-2</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="4"/>
-        <v>1.7837871035428981E-2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="5"/>
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3996,16 +3996,16 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
+        <f t="shared" si="5"/>
+        <v>-169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
         <f t="shared" si="6"/>
-        <v>169827.98000000045</v>
-      </c>
-      <c r="O32" s="5">
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
         <f t="shared" si="7"/>
-        <v>2.7581118653977402E-2</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="8"/>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -4020,15 +4020,15 @@
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>7418835.2699990273</v>
+        <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
         <f t="shared" si="1"/>
-        <v>7.9969930789269058E-3</v>
+        <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -4038,15 +4038,15 @@
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>2602486.5199999809</v>
+        <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
+        <f t="shared" si="8"/>
+        <v>-2.6564903115433454E-3</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="4"/>
-        <v>2.6564903115433454E-3</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="5"/>
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -4055,16 +4055,16 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
+        <f t="shared" si="5"/>
+        <v>-5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
         <f t="shared" si="6"/>
-        <v>5456610.5900000334</v>
-      </c>
-      <c r="O33" s="5">
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="7"/>
-        <v>5.5141067323084929E-3</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="8"/>
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4079,11 +4079,11 @@
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>79341.779999999795</v>
+        <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
         <f t="shared" si="1"/>
-        <v>1.8939149738619768E-2</v>
+        <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
@@ -4097,15 +4097,15 @@
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>213011.23000001023</v>
+        <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.8961345561534093E-2</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="4"/>
-        <v>4.8961345561534093E-2</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="5"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -4114,16 +4114,16 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
         <f t="shared" si="6"/>
-        <v>115798.49000000022</v>
-      </c>
-      <c r="O34" s="5">
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="7"/>
-        <v>2.6647296115611244E-2</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="8"/>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -4159,30 +4159,30 @@
         <v>0</v>
       </c>
       <c r="J35" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="5"/>
-        <v>48</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="5">
+      <c r="P35">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="8"/>
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -4197,15 +4197,15 @@
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>62776.72000000102</v>
+        <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="1"/>
-        <v>7.8647857679780775E-2</v>
+        <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -4215,15 +4215,15 @@
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>157733.05000000098</v>
+        <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="4"/>
-        <v>0.17551246244575608</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -4232,16 +4232,16 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
+        <f t="shared" si="5"/>
+        <v>-101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
         <f t="shared" si="6"/>
-        <v>101084.71000000101</v>
-      </c>
-      <c r="O36" s="5">
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
         <f t="shared" si="7"/>
-        <v>0.11509132414892521</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -4256,15 +4256,15 @@
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>82352.260000010021</v>
+        <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="1"/>
-        <v>3.9444515758219188E-2</v>
+        <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -4274,15 +4274,15 @@
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
-        <v>110256.79000000004</v>
+        <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.9460250314014013E-2</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="4"/>
-        <v>4.9460250314014013E-2</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -4291,16 +4291,16 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
+        <f t="shared" si="5"/>
+        <v>-188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
         <f t="shared" si="6"/>
-        <v>188181.66000000015</v>
-      </c>
-      <c r="O37" s="5">
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
         <f t="shared" si="7"/>
-        <v>8.1928538464887526E-2</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="8"/>
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4315,15 +4315,15 @@
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>16630.180000000051</v>
+        <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
         <f t="shared" si="1"/>
-        <v>1.9443680579913542E-2</v>
+        <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -4333,15 +4333,15 @@
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
-        <v>39348.040000000037</v>
+        <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.9631735620585316E-2</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="4"/>
-        <v>4.9631735620585316E-2</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -4350,16 +4350,16 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
+        <f t="shared" si="5"/>
+        <v>-136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
         <f t="shared" si="6"/>
-        <v>136.73999999999069</v>
-      </c>
-      <c r="O38" s="5">
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
         <f t="shared" si="7"/>
-        <v>1.7580354847003174E-4</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="8"/>
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -4374,15 +4374,15 @@
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>70791.13</v>
+        <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
         <f t="shared" si="1"/>
-        <v>8.008952370177623E-2</v>
+        <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -4392,15 +4392,15 @@
       </c>
       <c r="I39">
         <f t="shared" si="3"/>
-        <v>180157.72000000998</v>
+        <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
+        <f t="shared" si="8"/>
+        <v>-0.13918241656366656</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="4"/>
-        <v>0.13918241656366656</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -4409,16 +4409,16 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
+        <f t="shared" si="5"/>
+        <v>-79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
         <f t="shared" si="6"/>
-        <v>79036.1300000099</v>
-      </c>
-      <c r="O39" s="5">
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
         <f t="shared" si="7"/>
-        <v>4.4919653310605226E-2</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4433,15 +4433,15 @@
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>816758.14000009745</v>
+        <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
         <f t="shared" si="1"/>
-        <v>2.1279773539092578E-2</v>
+        <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -4451,15 +4451,15 @@
       </c>
       <c r="I40">
         <f t="shared" si="3"/>
-        <v>1869659.8100000992</v>
+        <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.6782546934937892E-2</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="4"/>
-        <v>4.6782546934937892E-2</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="5"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -4468,16 +4468,16 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
+        <f t="shared" si="5"/>
+        <v>-610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
         <f t="shared" si="6"/>
-        <v>610436.29000010341</v>
-      </c>
-      <c r="O40" s="5">
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
         <f t="shared" si="7"/>
-        <v>1.5178676768608648E-2</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="8"/>
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -4492,15 +4492,15 @@
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>184239.79000001028</v>
+        <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
         <f t="shared" si="1"/>
-        <v>4.0110550149132493E-2</v>
+        <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -4510,15 +4510,15 @@
       </c>
       <c r="I41">
         <f t="shared" si="3"/>
-        <v>133456.33000001032</v>
+        <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
+        <f t="shared" si="8"/>
+        <v>-2.6221894095689226E-2</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="4"/>
-        <v>2.6221894095689226E-2</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="5"/>
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -4527,16 +4527,16 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
+        <f t="shared" si="5"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
         <f t="shared" si="6"/>
-        <v>82077.349999999627</v>
-      </c>
-      <c r="O41" s="5">
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
         <f t="shared" si="7"/>
-        <v>1.7099804162586642E-2</v>
-      </c>
-      <c r="P41">
-        <f t="shared" si="8"/>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -4551,15 +4551,15 @@
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>41624.320001006126</v>
+        <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
         <f t="shared" si="1"/>
-        <v>2.2070943135841053E-4</v>
+        <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -4569,15 +4569,15 @@
       </c>
       <c r="I42">
         <f t="shared" si="3"/>
-        <v>2375266.6899999976</v>
+        <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
+        <f t="shared" si="8"/>
+        <v>-1.1928203241796942E-2</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="4"/>
-        <v>1.1928203241796942E-2</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="5"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -4586,16 +4586,16 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
+        <f t="shared" si="5"/>
+        <v>-36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
         <f t="shared" si="6"/>
-        <v>36.250001013278961</v>
-      </c>
-      <c r="O42" s="5">
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
         <f t="shared" si="7"/>
-        <v>1.8129115815929696E-7</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="8"/>
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -4610,15 +4610,15 @@
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>166754.16999999993</v>
+        <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
         <f t="shared" si="1"/>
-        <v>2.0497353541313264E-2</v>
+        <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -4628,15 +4628,15 @@
       </c>
       <c r="I43">
         <f t="shared" si="3"/>
-        <v>389327.98000000045</v>
+        <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.5477990374731388E-2</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="4"/>
-        <v>4.5477990374731388E-2</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="5"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -4645,16 +4645,16 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
+        <f t="shared" si="5"/>
+        <v>-346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
         <f t="shared" si="6"/>
-        <v>346517.43000000995</v>
-      </c>
-      <c r="O43" s="5">
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
         <f t="shared" si="7"/>
-        <v>4.0778750220654303E-2</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -4669,15 +4669,15 @@
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>294095.62000000104</v>
+        <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
         <f t="shared" si="1"/>
-        <v>9.7760750186150751E-3</v>
+        <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -4687,15 +4687,15 @@
       </c>
       <c r="I44">
         <f t="shared" si="3"/>
-        <v>246988.51999999955</v>
+        <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
+        <f t="shared" si="8"/>
+        <v>-7.9569249404813532E-3</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="4"/>
-        <v>7.9569249404813532E-3</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="5"/>
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -4704,16 +4704,16 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
+        <f t="shared" si="5"/>
+        <v>-58.75</v>
+      </c>
+      <c r="O44" s="5">
         <f t="shared" si="6"/>
-        <v>58.75</v>
-      </c>
-      <c r="O44" s="5">
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
         <f t="shared" si="7"/>
-        <v>1.8780648419868168E-6</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="8"/>
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -4728,15 +4728,15 @@
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>712015.95000009984</v>
+        <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
         <f t="shared" si="1"/>
-        <v>1.287514194887851E-2</v>
+        <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -4746,15 +4746,15 @@
       </c>
       <c r="I45">
         <f t="shared" si="3"/>
-        <v>2197246.0400001034</v>
+        <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.8689222111488959E-2</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="4"/>
-        <v>3.8689222111488959E-2</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -4763,16 +4763,16 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
+        <f t="shared" si="5"/>
+        <v>-640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
         <f t="shared" si="6"/>
-        <v>640550.34000010043</v>
-      </c>
-      <c r="O45" s="5">
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="7"/>
-        <v>1.1432866237947358E-2</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="8"/>
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4787,15 +4787,15 @@
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>777.57000000000698</v>
+        <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
         <f t="shared" si="1"/>
-        <v>3.0010420686993711E-3</v>
+        <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -4805,15 +4805,15 @@
       </c>
       <c r="I46">
         <f t="shared" si="3"/>
-        <v>8597.090000000986</v>
+        <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.2319887218048821E-2</v>
+      </c>
+      <c r="K46">
         <f t="shared" si="4"/>
-        <v>3.2319887218048821E-2</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="5"/>
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -4822,16 +4822,16 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
+        <f t="shared" si="5"/>
+        <v>-12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
         <f t="shared" si="6"/>
-        <v>12346.840000000986</v>
-      </c>
-      <c r="O46" s="5">
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
         <f t="shared" si="7"/>
-        <v>4.6225533508053113E-2</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="8"/>
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4846,15 +4846,15 @@
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>12273.280000001192</v>
+        <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
         <f t="shared" si="1"/>
-        <v>1.7435939690898361E-4</v>
+        <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -4864,15 +4864,15 @@
       </c>
       <c r="I47">
         <f t="shared" si="3"/>
-        <v>24458.340000003576</v>
+        <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.3291600310348285E-4</v>
+      </c>
+      <c r="K47">
         <f t="shared" si="4"/>
-        <v>3.3291600310348285E-4</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="5"/>
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -4881,16 +4881,16 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
+        <f t="shared" si="5"/>
+        <v>-21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
         <f t="shared" si="6"/>
-        <v>21970.820000097156</v>
-      </c>
-      <c r="O47" s="5">
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
         <f t="shared" si="7"/>
-        <v>2.9266019117572752E-4</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="8"/>
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4905,15 +4905,15 @@
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>209747.43000000995</v>
+        <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
         <f t="shared" si="1"/>
-        <v>3.1133192323107857E-2</v>
+        <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4923,15 +4923,15 @@
       </c>
       <c r="I48">
         <f t="shared" si="3"/>
-        <v>292627.44000000041</v>
+        <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
+        <f t="shared" si="8"/>
+        <v>-4.0559890224125802E-2</v>
+      </c>
+      <c r="K48">
         <f t="shared" si="4"/>
-        <v>4.0559890224125802E-2</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="5"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4940,16 +4940,16 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
+        <f t="shared" si="5"/>
+        <v>-407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
         <f t="shared" si="6"/>
-        <v>407449.76000001002</v>
-      </c>
-      <c r="O48" s="5">
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
         <f t="shared" si="7"/>
-        <v>5.5893132870587676E-2</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="8"/>
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4964,15 +4964,15 @@
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>1700.570000000007</v>
+        <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
         <f t="shared" si="1"/>
-        <v>1.8444360086767971E-2</v>
+        <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4982,33 +4982,33 @@
       </c>
       <c r="I49">
         <f t="shared" si="3"/>
-        <v>7133.1199999999953</v>
+        <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
+        <f t="shared" si="8"/>
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
         <f t="shared" si="4"/>
-        <v>6.9523586744639335E-2</v>
-      </c>
-      <c r="K49">
+        <v>39</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="5">
+      <c r="P49">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="8"/>
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -5044,12 +5044,12 @@
         <v>0</v>
       </c>
       <c r="J50" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="5"/>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -5058,16 +5058,16 @@
         <v>843200</v>
       </c>
       <c r="N50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="5">
+      <c r="P50">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="8"/>
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -5082,15 +5082,15 @@
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>110074.66000000946</v>
+        <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
         <f t="shared" si="1"/>
-        <v>1.2785255822058129E-2</v>
+        <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -5100,15 +5100,15 @@
       </c>
       <c r="I51">
         <f t="shared" si="3"/>
-        <v>326440.38000000082</v>
+        <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
+        <f t="shared" si="8"/>
+        <v>-3.6573903982970231E-2</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="4"/>
-        <v>3.6573903982970231E-2</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="5"/>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -5117,16 +5117,16 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
+        <f t="shared" si="5"/>
+        <v>-98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
         <f t="shared" si="6"/>
-        <v>98056.689999999478</v>
-      </c>
-      <c r="O51" s="5">
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="7"/>
-        <v>1.1100045280114048E-2</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="8"/>
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5141,15 +5141,15 @@
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>196315.20000000019</v>
+        <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
         <f t="shared" si="1"/>
-        <v>8.009596083231342E-2</v>
+        <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -5159,15 +5159,15 @@
       </c>
       <c r="I52">
         <f t="shared" si="3"/>
-        <v>236027.12000000011</v>
+        <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
+        <f t="shared" si="8"/>
+        <v>-9.6704683082722218E-2</v>
+      </c>
+      <c r="K52">
         <f t="shared" si="4"/>
-        <v>9.6704683082722218E-2</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="5"/>
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -5176,16 +5176,16 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
+        <f t="shared" si="5"/>
+        <v>-264764.74</v>
+      </c>
+      <c r="O52" s="5">
         <f t="shared" si="6"/>
-        <v>264764.74</v>
-      </c>
-      <c r="O52" s="5">
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
         <f t="shared" si="7"/>
-        <v>0.11404408166781529</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="8"/>
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -5213,15 +5213,15 @@
       </c>
       <c r="B56">
         <f>VLOOKUP($A56,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
-        <v>36209.630000000005</v>
+        <v>-36209.630000000005</v>
       </c>
       <c r="C56">
         <f t="shared" ref="C56:D61" si="9">VLOOKUP($A56,$A$2:$P$52,MATCH(C$55,$A$1:$P$1,0),FALSE)</f>
-        <v>27292.159999999974</v>
+        <v>-27292.159999999974</v>
       </c>
       <c r="D56">
         <f t="shared" si="9"/>
-        <v>9181.0800000000163</v>
+        <v>-9181.0800000000163</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="D57">
         <f t="shared" si="9"/>
-        <v>311228.08999999997</v>
+        <v>-311228.08999999997</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -5247,15 +5247,15 @@
       </c>
       <c r="B58">
         <f>VLOOKUP($A58,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
-        <v>149396.10000000987</v>
+        <v>-149396.10000000987</v>
       </c>
       <c r="C58">
         <f t="shared" si="9"/>
-        <v>189254.06000000006</v>
+        <v>-189254.06000000006</v>
       </c>
       <c r="D58">
         <f t="shared" si="9"/>
-        <v>374962.91000000015</v>
+        <v>-374962.91000000015</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -5264,15 +5264,15 @@
       </c>
       <c r="B59">
         <f t="shared" si="10"/>
-        <v>12230.810000000056</v>
+        <v>-12230.810000000056</v>
       </c>
       <c r="C59">
         <f t="shared" si="9"/>
-        <v>45485.580000000075</v>
+        <v>-45485.580000000075</v>
       </c>
       <c r="D59">
         <f t="shared" si="9"/>
-        <v>72.879999999888241</v>
+        <v>-72.879999999888241</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -5281,15 +5281,15 @@
       </c>
       <c r="B60">
         <f t="shared" si="10"/>
-        <v>4950.4699999999721</v>
+        <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
         <f t="shared" si="9"/>
-        <v>8005.7900000010268</v>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
         <f t="shared" si="9"/>
-        <v>1724.9000000000233</v>
+        <v>-1724.9000000000233</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -5298,15 +5298,15 @@
       </c>
       <c r="B61">
         <f t="shared" si="10"/>
-        <v>184239.79000001028</v>
+        <v>-184239.79000001028</v>
       </c>
       <c r="C61">
         <f t="shared" si="9"/>
-        <v>133456.33000001032</v>
+        <v>-133456.33000001032</v>
       </c>
       <c r="D61">
         <f t="shared" si="9"/>
-        <v>82077.349999999627</v>
+        <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -5338,11 +5338,11 @@
       </c>
       <c r="C65" cm="1">
         <f t="array" ref="C65">_xlfn.XLOOKUP(A56, A:A, I:I, NA)</f>
-        <v>27292.159999999974</v>
+        <v>-27292.159999999974</v>
       </c>
       <c r="D65" cm="1">
         <f t="array" ref="D65">_xlfn.XLOOKUP(A56, A:A, N:N, NA)</f>
-        <v>9181.0800000000163</v>
+        <v>-9181.0800000000163</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="D66" cm="1">
         <f t="array" ref="D66">_xlfn.XLOOKUP(A57, A:A, N:N, NA)</f>
-        <v>311228.08999999997</v>
+        <v>-311228.08999999997</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -5368,15 +5368,15 @@
       </c>
       <c r="B67" cm="1">
         <f t="array" ref="B67">_xlfn.XLOOKUP(A58, A:A, D:D, NA)</f>
-        <v>149396.10000000987</v>
+        <v>-149396.10000000987</v>
       </c>
       <c r="C67" cm="1">
         <f t="array" ref="C67">_xlfn.XLOOKUP(A58, A:A, I:I, NA)</f>
-        <v>189254.06000000006</v>
+        <v>-189254.06000000006</v>
       </c>
       <c r="D67" cm="1">
         <f t="array" ref="D67">_xlfn.XLOOKUP(A58, A:A, N:N, NA)</f>
-        <v>374962.91000000015</v>
+        <v>-374962.91000000015</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -5385,15 +5385,15 @@
       </c>
       <c r="B68" cm="1">
         <f t="array" ref="B68">_xlfn.XLOOKUP(A59, A:A, D:D, NA)</f>
-        <v>12230.810000000056</v>
+        <v>-12230.810000000056</v>
       </c>
       <c r="C68" cm="1">
         <f t="array" ref="C68">_xlfn.XLOOKUP(A59, A:A, I:I, NA)</f>
-        <v>45485.580000000075</v>
+        <v>-45485.580000000075</v>
       </c>
       <c r="D68" cm="1">
         <f t="array" ref="D68">_xlfn.XLOOKUP(A59, A:A, N:N, NA)</f>
-        <v>72.879999999888241</v>
+        <v>-72.879999999888241</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,15 +5402,15 @@
       </c>
       <c r="B69" cm="1">
         <f t="array" ref="B69">_xlfn.XLOOKUP(A60, A:A, D:D, NA)</f>
-        <v>4950.4699999999721</v>
+        <v>-4950.4699999999721</v>
       </c>
       <c r="C69" cm="1">
         <f t="array" ref="C69">_xlfn.XLOOKUP(A60, A:A, I:I, NA)</f>
-        <v>8005.7900000010268</v>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="D69" cm="1">
         <f t="array" ref="D69">_xlfn.XLOOKUP(A60, A:A, N:N, NA)</f>
-        <v>1724.9000000000233</v>
+        <v>-1724.9000000000233</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -5419,15 +5419,15 @@
       </c>
       <c r="B70" cm="1">
         <f t="array" ref="B70">_xlfn.XLOOKUP(A61, A:A, D:D, NA)</f>
-        <v>184239.79000001028</v>
+        <v>-184239.79000001028</v>
       </c>
       <c r="C70" cm="1">
         <f t="array" ref="C70">_xlfn.XLOOKUP(A61, A:A, I:I, NA)</f>
-        <v>133456.33000001032</v>
+        <v>-133456.33000001032</v>
       </c>
       <c r="D70" cm="1">
         <f t="array" ref="D70">_xlfn.XLOOKUP(A61, A:A, N:N, NA)</f>
-        <v>82077.349999999627</v>
+        <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -5455,15 +5455,15 @@
       </c>
       <c r="B74">
         <f>INDEX(D:D, MATCH(A56, A:A, 0))</f>
-        <v>36209.630000000005</v>
+        <v>-36209.630000000005</v>
       </c>
       <c r="C74">
         <f>INDEX(I:I, MATCH(A56, A:A, 0))</f>
-        <v>27292.159999999974</v>
+        <v>-27292.159999999974</v>
       </c>
       <c r="D74">
         <f>INDEX(N:N, MATCH(A56, A:A, 0))</f>
-        <v>9181.0800000000163</v>
+        <v>-9181.0800000000163</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
       </c>
       <c r="D75">
         <f t="shared" ref="D75:D79" si="13">INDEX(N:N, MATCH(A57, A:A, 0))</f>
-        <v>311228.08999999997</v>
+        <v>-311228.08999999997</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,15 +5489,15 @@
       </c>
       <c r="B76">
         <f t="shared" si="11"/>
-        <v>149396.10000000987</v>
+        <v>-149396.10000000987</v>
       </c>
       <c r="C76">
         <f t="shared" si="12"/>
-        <v>189254.06000000006</v>
+        <v>-189254.06000000006</v>
       </c>
       <c r="D76">
         <f t="shared" si="13"/>
-        <v>374962.91000000015</v>
+        <v>-374962.91000000015</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -5506,15 +5506,15 @@
       </c>
       <c r="B77">
         <f t="shared" si="11"/>
-        <v>12230.810000000056</v>
+        <v>-12230.810000000056</v>
       </c>
       <c r="C77">
         <f t="shared" si="12"/>
-        <v>45485.580000000075</v>
+        <v>-45485.580000000075</v>
       </c>
       <c r="D77">
         <f t="shared" si="13"/>
-        <v>72.879999999888241</v>
+        <v>-72.879999999888241</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -5523,15 +5523,15 @@
       </c>
       <c r="B78">
         <f t="shared" si="11"/>
-        <v>4950.4699999999721</v>
+        <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
         <f t="shared" si="12"/>
-        <v>8005.7900000010268</v>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
         <f t="shared" si="13"/>
-        <v>1724.9000000000233</v>
+        <v>-1724.9000000000233</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -5540,15 +5540,15 @@
       </c>
       <c r="B79">
         <f t="shared" si="11"/>
-        <v>184239.79000001028</v>
+        <v>-184239.79000001028</v>
       </c>
       <c r="C79">
         <f t="shared" si="12"/>
-        <v>133456.33000001032</v>
+        <v>-133456.33000001032</v>
       </c>
       <c r="D79">
         <f t="shared" si="13"/>
-        <v>82077.349999999627</v>
+        <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed postive values to negative
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojns\Documents\DA8\Projects\budget_lookups-Jerspen175\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761D6E15-DA13-4B09-BC84-1C64E8AE4453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD26B5B-E856-477D-A1AF-941AB48E6BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="30" windowWidth="11955" windowHeight="20730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2111,8 +2111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>